<commit_message>
added all the files to git
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>bjdbj</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>heeba</t>
+  </si>
+  <si>
+    <t>anam</t>
   </si>
 </sst>
 </file>
@@ -359,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -387,6 +390,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>